<commit_message>
befor drop and fill
</commit_message>
<xml_diff>
--- a/doc/财务记录/XDM-I研发采购18年4月-6月.xlsx
+++ b/doc/财务记录/XDM-I研发采购18年4月-6月.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>元器件</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -110,6 +110,87 @@
   </si>
   <si>
     <t>https://item.taobao.com/item.htm?spm=a230r.1.14.32.26305edbojRamN&amp;id=18854347328&amp;ns=1&amp;abbucket=19#detail</t>
+  </si>
+  <si>
+    <t>制版费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>PCB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>制版费预付款</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>嘉利创</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>充值</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>200</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>手续费</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -455,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:G10"/>
+  <dimension ref="B1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -467,9 +548,15 @@
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="15.375" customWidth="1"/>
     <col min="6" max="6" width="42.375" customWidth="1"/>
+    <col min="8" max="8" width="24.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7">
+    <row r="1" spans="2:8">
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8">
       <c r="B2">
         <v>20180401</v>
       </c>
@@ -489,7 +576,7 @@
         <v>82.59</v>
       </c>
     </row>
-    <row r="3" spans="2:7">
+    <row r="3" spans="2:8">
       <c r="B3">
         <v>20180401</v>
       </c>
@@ -509,7 +596,7 @@
         <v>39.53</v>
       </c>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="2:8">
       <c r="B4">
         <v>20180402</v>
       </c>
@@ -529,7 +616,7 @@
         <v>42.58</v>
       </c>
     </row>
-    <row r="5" spans="2:7">
+    <row r="5" spans="2:8">
       <c r="B5">
         <v>20180403</v>
       </c>
@@ -549,10 +636,30 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="2:7">
+    <row r="6" spans="2:8">
+      <c r="B6">
+        <v>20180407</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6">
+        <v>202</v>
+      </c>
+      <c r="H6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8">
       <c r="G10">
         <f>SUM(G2:G9)</f>
-        <v>214.7</v>
+        <v>416.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>